<commit_message>
atualização de dado na planilha
</commit_message>
<xml_diff>
--- a/PD.xlsx
+++ b/PD.xlsx
@@ -241,10 +241,10 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.14"/>
@@ -371,9 +371,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
-        <v>39.9</v>
+        <v>30.9</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>8</v>

</xml_diff>